<commit_message>
modfiy in all page
</commit_message>
<xml_diff>
--- a/uploads/المصنف1.xlsx
+++ b/uploads/المصنف1.xlsx
@@ -16,13 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
-  <si>
-    <t>ابتهال</t>
-  </si>
-  <si>
-    <t>طالب عوده كاظم</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>رابعه</t>
   </si>
@@ -30,103 +24,43 @@
     <t>كلا</t>
   </si>
   <si>
-    <t xml:space="preserve">اديان </t>
-  </si>
-  <si>
-    <t>صالح نجم</t>
-  </si>
-  <si>
-    <t xml:space="preserve">اسراء </t>
-  </si>
-  <si>
-    <t>جواد كريم عطيه</t>
-  </si>
-  <si>
     <t>نعم</t>
   </si>
   <si>
-    <t>محسن هاشم</t>
-  </si>
-  <si>
-    <t>اسيا</t>
-  </si>
-  <si>
-    <t>امال</t>
-  </si>
-  <si>
-    <t xml:space="preserve">حسين جبر </t>
-  </si>
-  <si>
-    <t>جاسم محمد</t>
-  </si>
-  <si>
-    <t>ايات</t>
-  </si>
-  <si>
-    <t>ايمن</t>
-  </si>
-  <si>
-    <t>ايه لؤي</t>
-  </si>
-  <si>
-    <t>تاج الدين</t>
-  </si>
-  <si>
-    <t>تبارك</t>
-  </si>
-  <si>
-    <t xml:space="preserve">حسن </t>
-  </si>
-  <si>
-    <t>تهلوك</t>
-  </si>
-  <si>
-    <t>حاتم</t>
-  </si>
-  <si>
-    <t>كريم مخيلف</t>
-  </si>
-  <si>
-    <t>علي جبار</t>
-  </si>
-  <si>
-    <t>حسين سهيل</t>
-  </si>
-  <si>
-    <t>لؤي عبد العباس</t>
-  </si>
-  <si>
-    <t>سلمان</t>
-  </si>
-  <si>
-    <t>جاسم  محمد</t>
-  </si>
-  <si>
-    <t xml:space="preserve">حسين </t>
-  </si>
-  <si>
-    <t>علي عبود</t>
-  </si>
-  <si>
-    <t>جبار عبدالحسين</t>
-  </si>
-  <si>
-    <t>حيدر</t>
-  </si>
-  <si>
-    <t>رحمان عبد المحسن</t>
-  </si>
-  <si>
-    <t>قاسم صلال</t>
-  </si>
-  <si>
-    <t>دعاء</t>
-  </si>
-  <si>
-    <t>زيد</t>
-  </si>
-  <si>
-    <t>حميد</t>
+    <t>ابتهال طالب عوده كاظم</t>
+  </si>
+  <si>
+    <t>اديان صالح نجم</t>
+  </si>
+  <si>
+    <t>اسراء جواد كريم عطيه</t>
+  </si>
+  <si>
+    <t>اسيا محسن هاشم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">امال حسين جبر </t>
+  </si>
+  <si>
+    <t>ايات جاسم محمد</t>
+  </si>
+  <si>
+    <t>ايمن حاتم</t>
+  </si>
+  <si>
+    <t>ايه لؤي لؤي عبد العباس</t>
+  </si>
+  <si>
+    <t>تاج الدين حسين سهيل</t>
+  </si>
+  <si>
+    <t>تبارك علي جبار</t>
+  </si>
+  <si>
+    <t>حاتم كريم مخيلف</t>
+  </si>
+  <si>
+    <t>حسن تهلوك</t>
   </si>
 </sst>
 </file>
@@ -465,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,16 +415,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -498,251 +429,131 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>